<commit_message>
Commit Latest changes related to Data provider
</commit_message>
<xml_diff>
--- a/FreeCRMAutmation/src/main/resources/FreeCRMData.xlsx
+++ b/FreeCRMAutmation/src/main/resources/FreeCRMData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="7860" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="7860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="ContactSheet" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:K25"/>
+  <oleSize ref="A1:F25"/>
 </workbook>
 </file>
 
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Commit changes of the data provider mismatch
</commit_message>
<xml_diff>
--- a/FreeCRMAutmation/src/main/resources/FreeCRMData.xlsx
+++ b/FreeCRMAutmation/src/main/resources/FreeCRMData.xlsx
@@ -8,16 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="ContactSheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="ContactSheet" sheetId="3" r:id="rId3"/>
+    <sheet name="ContactSheet" sheetId="2" r:id="rId2"/>
+    <sheet name="ContactSheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:F25"/>
+  <oleSize ref="A1:K25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>BirthDay Certificate</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Sri</t>
   </si>
 </sst>
 </file>
@@ -573,39 +579,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="19.77734375" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" customWidth="1"/>
-    <col min="12" max="12" width="21.5546875" customWidth="1"/>
-    <col min="13" max="13" width="18.5546875" customWidth="1"/>
-    <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="12.88671875" customWidth="1"/>
-    <col min="19" max="19" width="15.88671875" customWidth="1"/>
-    <col min="20" max="20" width="23.6640625" customWidth="1"/>
-    <col min="21" max="21" width="20.44140625" customWidth="1"/>
-    <col min="22" max="22" width="17.6640625" customWidth="1"/>
-    <col min="23" max="23" width="19.21875" customWidth="1"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" customWidth="1"/>
+    <col min="13" max="13" width="21.5546875" customWidth="1"/>
+    <col min="14" max="14" width="18.5546875" customWidth="1"/>
+    <col min="15" max="15" width="25" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="18" max="18" width="12.88671875" customWidth="1"/>
+    <col min="20" max="20" width="15.88671875" customWidth="1"/>
+    <col min="21" max="21" width="23.6640625" customWidth="1"/>
+    <col min="22" max="22" width="20.44140625" customWidth="1"/>
+    <col min="23" max="23" width="17.6640625" customWidth="1"/>
+    <col min="24" max="24" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -613,70 +619,73 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>37</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>39</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>43</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>44</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>45</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -684,74 +693,77 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>32</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>34</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>38</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>40</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>42</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>500072</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>26</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>46</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit Changes to Data provider
</commit_message>
<xml_diff>
--- a/FreeCRMAutmation/src/main/resources/FreeCRMData.xlsx
+++ b/FreeCRMAutmation/src/main/resources/FreeCRMData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="7860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="7860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,20 +771,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="2" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -792,10 +792,13 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -803,6 +806,9 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed with Data provider with two rows.
</commit_message>
<xml_diff>
--- a/FreeCRMAutmation/src/main/resources/FreeCRMData.xlsx
+++ b/FreeCRMAutmation/src/main/resources/FreeCRMData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="7860" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14232" windowHeight="7860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="ContactSheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:K25"/>
+  <oleSize ref="E1:R25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="54">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Sri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latha1 </t>
+  </si>
+  <si>
+    <t>Singh1</t>
+  </si>
+  <si>
+    <t>Sri1</t>
   </si>
 </sst>
 </file>
@@ -582,7 +591,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="R1" sqref="R1:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,10 +780,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +793,7 @@
     <col min="4" max="4" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -797,8 +806,68 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -811,8 +880,150 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2">
+        <v>500072</v>
+      </c>
+      <c r="V2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3">
+        <v>500072</v>
+      </c>
+      <c r="V3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="J3" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
+    <hyperlink ref="F3" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>